<commit_message>
wip: concentration check feature
</commit_message>
<xml_diff>
--- a/relatorio_proc_dados.xlsx
+++ b/relatorio_proc_dados.xlsx
@@ -58,13 +58,13 @@
     <t>CLORETO DE SÓDIO;GLICOSE</t>
   </si>
   <si>
-    <t>1000ML</t>
-  </si>
-  <si>
-    <t>250ML</t>
-  </si>
-  <si>
-    <t>500ML</t>
+    <t>1000ml</t>
+  </si>
+  <si>
+    <t>250ml</t>
+  </si>
+  <si>
+    <t>500ml</t>
   </si>
   <si>
     <t>JP</t>

</xml_diff>

<commit_message>
refactor: improve modularity and maintainability of the Test class
</commit_message>
<xml_diff>
--- a/relatorio_proc_dados.xlsx
+++ b/relatorio_proc_dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Item</t>
   </si>
@@ -43,34 +43,145 @@
     <t>Tempo Decorrido</t>
   </si>
   <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>CLORETO DE SÓDIO;GLICOSE</t>
-  </si>
-  <si>
-    <t>1000ml</t>
-  </si>
-  <si>
-    <t>250ml</t>
-  </si>
-  <si>
-    <t>500ml</t>
-  </si>
-  <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+    <t>HEPARINA SODICA SUBCUT 5000UI</t>
+  </si>
+  <si>
+    <t>PROMETAZINA 25MG, CLORIDRATO</t>
+  </si>
+  <si>
+    <t>HALOPERIDOL 5MG</t>
+  </si>
+  <si>
+    <t>CLORPROMAZINA 40MG/ML SOL ORAL</t>
+  </si>
+  <si>
+    <t>HALOPERIDOL 2MG/ML SOL ORAL</t>
+  </si>
+  <si>
+    <t>CLORPROMAZINA 25MG</t>
+  </si>
+  <si>
+    <t>CODEINA 30MG</t>
+  </si>
+  <si>
+    <t>IMIPRAMINA 25MG</t>
+  </si>
+  <si>
+    <t>RISPERIDONA 3MG</t>
+  </si>
+  <si>
+    <t>RISPERIDONA 1MG</t>
+  </si>
+  <si>
+    <t>LEVOMEPROMAZINA 4% GOTAS</t>
+  </si>
+  <si>
+    <t>LIDOCAINA 2% C/ VASO CONSTRITO</t>
+  </si>
+  <si>
+    <t>NITRATO DE CERIO +SULFADIAZINA</t>
+  </si>
+  <si>
+    <t>COLAGENASE+CLORAFENICOL POMADA 30g</t>
+  </si>
+  <si>
+    <t>sodica;heparina</t>
+  </si>
+  <si>
+    <t>PROMETAZINA</t>
+  </si>
+  <si>
+    <t>HALOPERIDOL</t>
+  </si>
+  <si>
+    <t>clorpromazina</t>
+  </si>
+  <si>
+    <t>codeina</t>
+  </si>
+  <si>
+    <t>imipramina</t>
+  </si>
+  <si>
+    <t>RISPERIDONA</t>
+  </si>
+  <si>
+    <t>levomepromazina</t>
+  </si>
+  <si>
+    <t>LIDOCAÍNA</t>
+  </si>
+  <si>
+    <t>NITRATO DE CERIO;SULFADIAZINA</t>
+  </si>
+  <si>
+    <t>COLAGENASE</t>
+  </si>
+  <si>
+    <t>5000ui</t>
+  </si>
+  <si>
+    <t>25mg</t>
+  </si>
+  <si>
+    <t>5mg</t>
+  </si>
+  <si>
+    <t>40mg/ml</t>
+  </si>
+  <si>
+    <t>2mg/ml</t>
+  </si>
+  <si>
+    <t>30mg</t>
+  </si>
+  <si>
+    <t>3mg</t>
+  </si>
+  <si>
+    <t>1mg</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>Concentração não encontrada</t>
+  </si>
+  <si>
+    <t>30g</t>
+  </si>
+  <si>
+    <t>Cristália</t>
+  </si>
+  <si>
+    <t>Teuto</t>
+  </si>
+  <si>
+    <t>Cellera</t>
+  </si>
+  <si>
+    <t>Sanofi</t>
+  </si>
+  <si>
+    <t>Vitamedic</t>
+  </si>
+  <si>
+    <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+  </si>
+  <si>
+    <t>LABORATÓRIO TEUTO BRASILEIRO S/A</t>
+  </si>
+  <si>
+    <t>CELLERA FARMACÊUTICA S.A.</t>
+  </si>
+  <si>
+    <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
   </si>
 </sst>
 </file>
@@ -428,7 +539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,82 +576,282 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: bug from last commit fixed
</commit_message>
<xml_diff>
--- a/relatorio_proc_dados.xlsx
+++ b/relatorio_proc_dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="147">
   <si>
     <t>Item</t>
   </si>
@@ -40,85 +40,421 @@
     <t>PDF</t>
   </si>
   <si>
-    <t>ALBENDAZOL 40 MG/ML SUSPENSAO ORAL   - FRASCO COM 10 ML  - FRASCO COM 10 ML</t>
-  </si>
-  <si>
-    <t>AMOXICILINA 250MG/5ML SUSPENSAO ORAL 150ML</t>
-  </si>
-  <si>
-    <t>AMOXILINA + CLAVULANATO DE POTASSIO 50+12,5 MG/ML PO PARA SUSPENSAO ORAL</t>
-  </si>
-  <si>
-    <t>AMOXILINA + CLAVULANATO DE POTASSIO 500+125 MG COMPRIMIDO</t>
-  </si>
-  <si>
-    <t>AZITROMICINA 40 MG/ML (600 MG) PO PARA SUSPENSAO ORAL</t>
-  </si>
-  <si>
-    <t>DEXCLORFENIRAMINA MALEATO 2MG</t>
-  </si>
-  <si>
-    <t>DOXAZOSINA MESILATO 4MG</t>
-  </si>
-  <si>
-    <t>ALBENDAZOL</t>
-  </si>
-  <si>
-    <t>AMOXICILINA</t>
-  </si>
-  <si>
-    <t>CLAVULANATO DE POTÁSSIO</t>
-  </si>
-  <si>
-    <t>AZITROMICINA</t>
-  </si>
-  <si>
-    <t>DEXCLORFENIRAMINA</t>
-  </si>
-  <si>
-    <t>mesilato;doxazosina</t>
-  </si>
-  <si>
-    <t>40 mg/ml</t>
-  </si>
-  <si>
-    <t>250mg</t>
-  </si>
-  <si>
-    <t>5 mg/ml</t>
-  </si>
-  <si>
-    <t>125 mg</t>
-  </si>
-  <si>
-    <t>2mg</t>
-  </si>
-  <si>
-    <t>4mg</t>
-  </si>
-  <si>
-    <t>Geolab</t>
-  </si>
-  <si>
-    <t>Eurofarma</t>
-  </si>
-  <si>
-    <t>EMS</t>
-  </si>
-  <si>
-    <t>Pharlab</t>
+    <t xml:space="preserve">DISPOSITIVO PARA INTRODUÇÃO EM ORGÃOS CORPORAIS PARA DRENAGEM DE FLUIDOS. (SECREÇÕES OU EXCREÇÕES), FEITA EM PVC ATÓXICO SILICONADO, ESTÉRIL DESCARTÁVEL (USO ÚNICO), EMBALADAS INDIVIDUALMENTE, POSSUI A FINALIDADE DE ESVAZIAR A BEXIGA, TODAS AS SONDAS DESCARTÁVEIS SÃO COMPOSTAS DE TUBO DE PVC ATÓXICO FLEXÍVEL COM MODELO DE FURAÇÃO ESPECÍFICA (2 FUROS) E CONECTOR COM TAMPA. INFORMAÇÕES SOBRE PROCEDÊNCIA E VALIDADE IMPRESSAS EMBALAGEM, GARANTIA CONTRA DEFEITOS DE FABRICAÇÃO OU MATERIAIS. (SONDA URETAL Nº12).. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPOSITIVO PARA INTRODUÇÃO EM ÓRGÃOS CORPORAIS PARA DRENAGEM DE FLUIDOS. (SECREÇÕES OU EXCREÇÕES) FEITA EM PVC ATÓXICO SILICONADO, ESTÉRIL DESCARTÁVEL (USO ÚNICO), EMBALADAS INDIVIDUALMENTE, POSSUI A FINALIDADE DE ESVAZIAR A BEXIGA, TODAS AS SONDAS DESCARTÁVEIS SÃO COMPOSTAS DE TUBO DE PVC ATÓXICO FLEXÍVEL COM MODELO DE FURAÇÃO ESPECÍFICA (2 FUROS) E CONECTOR COM TAMPA. INFORMAÇÕES SOBRE PROCEDÊNCIA E VALIDADE IMPRESSAS EMBALAGEM, GARANTIA CONTRA DEFEITOS DE FABRICAÇÃO OU MATERIAIS. (SONDA URETAL Nº10.). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRASCO FRACIONADO PARA ADMINISTRAÇÃO DE SOLUÇÃO ENTERAIS, CAPACIDADE DE 500ML. PERMITE TRATAMENTO TÉRMICO (AQUECIMENTO, RESFRIAMENTO) DE SOLUÇÕES, COM DISPOSITIVO PARA FIXAÇÃO EM SUPORTE.( FRASCO PARA ALIMENTAÇÃO 500ML).. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPOSITIVO PARA A ADMINISTRAÇÃO. (ACESSO ENTERAL) DE FLUIDOS ALIMENTO, MEDICAMENTO, ÁGUA, NUTRIENTES, COMPOSTOS LIPÍDICOS NHPP RTC, CONTIDOS EM FRASCOS PARA O SISTEMA GASTROINTESTINAL (ACESSO ENTERAL NO PACIENTE).(EQUIPO PARA NUTRIÇÃO ENTERAL).. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIRAGLUTIDA INSULINA DEGLUDECA 100 U/ML + 3,6 MG/ML SOL INJ CT X 1 CAR VD. TRANS X 3 ML + 1 SIST APLIC PLAS (INSULINA XULTOPHY). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSULINA ASPARTE 100 U/ML SOL INJ CT 1 CAR VD TRABS X 3 ML + 1 SIST APLIC PLAS. FLEXPEN INSULINA FIASP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO DE METFORMINA 1G COM REV EST BL AL PLAS TRANS X 30 GLIFAGE. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO DE METFORMINA 750MG COM REV EST BL AL PLAS TRANS X 30 GLIFAGE. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO DE METFORMINA 500MG COM REV EST BL AL PLAS TRANS X 30 GLIFAGE. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO DE METFORMINA 850MG COM REV EST BL AL PLAS TRANS X 30 GLIFAGE. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOZAPINA 25MG COM CT BL AL PLAS TRANS X 30. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOBESILATO DE CLACIO 500MG CAP DURA CT BL AL AL X 30 DOBEVEN. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIMESLATO DE LISDEXANFETAMINA 70MG CAP DURA CT FR PLAS OPC X 28 VENVANSE. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIMESLATO DE LISDEXANFETAMINA 50MG CAP DURA CT FR PLAS OPC X28 VENVANSE. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BACITRACINA SULFATO DE NEOMICINA 5,0 MG/G + 250 UI/G POM DERM CT BG AL X 10G. NEOMICINA POMADA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OXCARBAZEPINA 60 MG/ML SUS OR CT FR VD AMB X 100ML + 2 SE DOS TRILEPTAL SUS. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMIPRIL 10MG COM CT BL AL X 30 NAPRIX 10MG. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMIPRIL BESILATO DE ANLODIPINO 10MG + 10MG CAP GEL DURA CT FR PLAS X 30 NAPRIX. 10MG+10MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMIPRIL BESILATO DE ANLODIPINO 5MG + 5MG CAP GEL DURA CT FR PLAS X 30 NAPRIX. 10MG+5MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUPRENORFINA 10MG ADES TRANSD CT ENV X 2RESTIVA 10MG. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIDROCLOROTIAZIDA TELMISARTANA 80MG + 25MG COM CT BL AL/AL X 30. MICARDIS HCT 80/12,5MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALSARTANA  HIDROCLOROTIAZIDA BESILATO DE AN 160,00+12,50+10,00MG. COM REV CT BL AL AL X 2/ EXFORGE 160MG + 12,5MG+10MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALSARTANA  HIDROCLOROTIAZIDA BESILATO ANLODIPINO 320,00+25,00+10,00. MG COM REV CT BL AL AL 28 EXFORGE 320MG+25MG+10MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALSARTANA SACUBITRIL 200MG COM REV CT BL AL AL X 60. ENTRESTO 200MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALSARTANA SACUBITRIL 50MG COM REV CT BL AL AL X 28. ENTRESTO 50MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALSARTANA SACUBITRIL 100MG COM REV CT BL AL AL X 60. ENTRESTO 100MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BESILATO DE ANLODIPINO PERINDOPRIL ARGININA 14MG + 10MG. COM CT TB PLAS PP OPC X 30 ACERTANLO 14MG/10MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BESILATO DE ANLODIPINO PERINDOPRIL ARGININA 7MG + 5MG. COM CT TB PLAS PP OPC X 30 ACERTANLO 7MG/5MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARIPIPRAZOL 1 MG/ML SUS OR CT FR PLAS PET AMB X 100ML + SER DOS ARISTAB. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO DE FEXOFENADINA ALLEGRA D DE PSEUDOEFEDRINA 60,0 + 120,0MG. COM REV LIB PROL CT BL AL PLAS PVC PE PVDC TRANS. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAIXA CONTENDO 50 TIRAS REAGENTES PARA DETECÇÃO DE GLICOSE SANGUÍNEA COMPATIVEIS. COM MONITOR DE GLICEMIA PERFORMA COMBO (INSUMOS PARA BOMBA DE INFUSÃO DE INSULINA COMPATÍVEL COM ACCU-CHEK).. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO DE MEMANTINA 10MG COM REV CT BL AL PLAS TRANS X30. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FENOFIBRATO 160MG COM REV CT BL AL PLAS PVC PE PVDC TRANS X30. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICLORIDRATO DE ZUCLOPENTIXOL CLOPIXOL 10MG. 10 MG COM REV CT BL AL PLAS TRNS X20. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO METFORMINA EMPAGLIFLOZINA 12,5+850MG COM REV CT BL AL PLAS PVC PCTFE. OPC X 60 JARDIANCE DUO 850MG+12,5MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLORIDRATO METFORMINA EMPAGLIFLOZINA 12,5+1000MG. COM REV CT BL AL PLAS PVC PCTFE OPC X60 JARDIANCE DUO 1000MG+12,5MG. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BROMOPRIDA 4MG/ML SOL OR CT FR GOT PLAS OPC X 20ML. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIDROCLOROTIAZIDA CANDESARTANA CILEXETILA 16MG +12,5MG. COM CT BL AL PLAS TRANS X30. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANDESARTANA CILEXETILA 16MG COM CT BL AL PLAS TRANS X30. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANDESARTANA CILEXETILA 8MG COM CT BL AL PLAS TRANS X 30. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMAGLUTIDA 1,34 MG/ML SOL INJ CT X 1 CAR VD TRANS X 1,5 ML + 1. SIST APLIC PLAS DOSES 0,25MG E 0,5MG + 6 AGULHAS NOVOFINE OZEMPIC. </t>
+  </si>
+  <si>
+    <t>fluido;forma;esteril</t>
+  </si>
+  <si>
+    <t>fluido;agua</t>
+  </si>
+  <si>
+    <t>INSULINA DEGLUDECA;LIRAGLUTIDA</t>
+  </si>
+  <si>
+    <t>INSULINA ASPARTE</t>
+  </si>
+  <si>
+    <t>CLORIDRATO DE METFORMINA</t>
+  </si>
+  <si>
+    <t>CLOZAPINA</t>
+  </si>
+  <si>
+    <t>besilato</t>
+  </si>
+  <si>
+    <t>lisdexanfetamina</t>
+  </si>
+  <si>
+    <t>SULFATO DE NEOMICINA;BACITRACINA;NEOMICINA</t>
+  </si>
+  <si>
+    <t>OXCARBAZEPINA</t>
+  </si>
+  <si>
+    <t>RAMIPRIL</t>
+  </si>
+  <si>
+    <t>BESILATO DE ANLODIPINO;RAMIPRIL</t>
+  </si>
+  <si>
+    <t>BUPRENORFINA</t>
+  </si>
+  <si>
+    <t>HIDROCLOROTIAZIDA;TELMISARTANA</t>
+  </si>
+  <si>
+    <t>HIDROCLOROTIAZIDA;VALSARTANA</t>
+  </si>
+  <si>
+    <t>VALSARTANA;SACUBITRIL</t>
+  </si>
+  <si>
+    <t>BESILATO DE ANLODIPINO;PERINDOPRIL ARGININA</t>
+  </si>
+  <si>
+    <t>ARIPIPRAZOL</t>
+  </si>
+  <si>
+    <t>CLORIDRATO DE FEXOFENADINA;PSEUDOEFEDRINA</t>
+  </si>
+  <si>
+    <t>GLICOSE</t>
+  </si>
+  <si>
+    <t>CLORIDRATO DE MEMANTINA</t>
+  </si>
+  <si>
+    <t>FENOFIBRATO</t>
+  </si>
+  <si>
+    <t>DICLORIDRATO DE ZUCLOPENTIXOL</t>
+  </si>
+  <si>
+    <t>EMPAGLIFLOZINA</t>
+  </si>
+  <si>
+    <t>BROMOPRIDA</t>
+  </si>
+  <si>
+    <t>CANDESARTANA CILEXETILA;HIDROCLOROTIAZIDA</t>
+  </si>
+  <si>
+    <t>CANDESARTANA CILEXETILA</t>
+  </si>
+  <si>
+    <t>SEMAGLUTIDA</t>
+  </si>
+  <si>
+    <t>Concentração não encontrada</t>
+  </si>
+  <si>
+    <t>500ml</t>
+  </si>
+  <si>
+    <t>6 mg/ml</t>
+  </si>
+  <si>
+    <t>3 ml</t>
+  </si>
+  <si>
+    <t>1g</t>
+  </si>
+  <si>
+    <t>750mg</t>
+  </si>
+  <si>
+    <t>500mg</t>
+  </si>
+  <si>
+    <t>850mg</t>
+  </si>
+  <si>
+    <t>25mg</t>
+  </si>
+  <si>
+    <t>70mg</t>
+  </si>
+  <si>
+    <t>50mg</t>
+  </si>
+  <si>
+    <t>0 mg</t>
+  </si>
+  <si>
+    <t>60 mg/ml</t>
+  </si>
+  <si>
+    <t>10mg</t>
+  </si>
+  <si>
+    <t>5mg</t>
+  </si>
+  <si>
+    <t>80mg</t>
+  </si>
+  <si>
+    <t>00mg</t>
+  </si>
+  <si>
+    <t>320mg</t>
+  </si>
+  <si>
+    <t>200mg</t>
+  </si>
+  <si>
+    <t>100mg</t>
+  </si>
+  <si>
+    <t>14mg</t>
+  </si>
+  <si>
+    <t>7mg</t>
+  </si>
+  <si>
+    <t>1 mg/ml</t>
+  </si>
+  <si>
+    <t>0mg</t>
+  </si>
+  <si>
+    <t>160mg</t>
+  </si>
+  <si>
+    <t>1000mg</t>
+  </si>
+  <si>
+    <t>4mg/ml</t>
+  </si>
+  <si>
+    <t>16mg</t>
+  </si>
+  <si>
+    <t>8mg</t>
+  </si>
+  <si>
+    <t>34 mg/ml</t>
+  </si>
+  <si>
+    <t>markmed</t>
+  </si>
+  <si>
+    <t>biobase</t>
+  </si>
+  <si>
+    <t>descarpack</t>
+  </si>
+  <si>
+    <t>novo nordisk</t>
+  </si>
+  <si>
+    <t>merck</t>
+  </si>
+  <si>
+    <t>viatriz</t>
+  </si>
+  <si>
+    <t>apsen</t>
+  </si>
+  <si>
+    <t>takeda</t>
+  </si>
+  <si>
+    <t>belfar</t>
+  </si>
+  <si>
+    <t>novartis</t>
+  </si>
+  <si>
+    <t>libbs</t>
+  </si>
+  <si>
+    <t>mundipharma</t>
+  </si>
+  <si>
+    <t>boehringer</t>
+  </si>
+  <si>
+    <t>servier</t>
+  </si>
+  <si>
+    <t>ache</t>
+  </si>
+  <si>
+    <t>sanofi</t>
+  </si>
+  <si>
+    <t>roche</t>
+  </si>
+  <si>
+    <t>geolab</t>
+  </si>
+  <si>
+    <t>abbott</t>
+  </si>
+  <si>
+    <t>lundbeck</t>
+  </si>
+  <si>
+    <t>airela</t>
+  </si>
+  <si>
+    <t>sandoz</t>
+  </si>
+  <si>
+    <t>NOVO NORDISK PRODUÇÃO FARMACÊUTICA DO BRASIL LTDA</t>
+  </si>
+  <si>
+    <t>MERCK S/A</t>
+  </si>
+  <si>
+    <t>APSEN FARMACEUTICA S/A</t>
+  </si>
+  <si>
+    <t>TAKEDA PHARMA LTDA</t>
+  </si>
+  <si>
+    <t>BELFAR LTDA</t>
+  </si>
+  <si>
+    <t>NOVARTIS BIOCIENCIAS S.A</t>
+  </si>
+  <si>
+    <t>LIBBS FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>MUNDIPHARMA BRASIL PRODUTOS MÉDICOS E FARMACÊUTICOS LTDA</t>
+  </si>
+  <si>
+    <t>BOEHRINGER INGELHEIM DO BRASIL QUÍMICA E FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>LABORATÓRIOS SERVIER DO BRASIL LTDA</t>
+  </si>
+  <si>
+    <t>ACHÉ LABORATÓRIOS FARMACÊUTICOS S.A</t>
+  </si>
+  <si>
+    <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>PRODUTOS ROCHE QUÍMICOS E FARMACÊUTICOS S.A.</t>
   </si>
   <si>
     <t>GEOLAB INDÚSTRIA FARMACÊUTICA S/A</t>
   </si>
   <si>
-    <t>EUROFARMA LABORATÓRIOS S.A.</t>
-  </si>
-  <si>
-    <t>EMS SIGMA PHARMA LTDA</t>
-  </si>
-  <si>
-    <t>PHARLAB INDÚSTRIA FARMACÊUTICA S.A.</t>
+    <t>ABBOTT LABORATÓRIOS DO BRASIL LTDA</t>
+  </si>
+  <si>
+    <t>LUNDBECK BRASIL LTDA</t>
+  </si>
+  <si>
+    <t>AIRELA INDÚSTRIA FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>SANDOZ DO BRASIL INDÚSTRIA FARMACÊUTICA LTDA</t>
   </si>
 </sst>
 </file>
@@ -476,7 +812,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -510,142 +846,822 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
         <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" t="s">
+        <v>127</v>
+      </c>
+      <c r="F38" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>65</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>66</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: extract checkpoint functionality into separate module
</commit_message>
<xml_diff>
--- a/relatorio_proc_dados.xlsx
+++ b/relatorio_proc_dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Item</t>
   </si>
@@ -40,34 +40,73 @@
     <t>PDF</t>
   </si>
   <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>CLORETO DE SÓDIO;GLICOSE</t>
-  </si>
-  <si>
-    <t>1000ml</t>
-  </si>
-  <si>
-    <t>250ml</t>
-  </si>
-  <si>
-    <t>500ml</t>
-  </si>
-  <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+    <t>RISPERIDONA 3MG</t>
+  </si>
+  <si>
+    <t>RISPERIDONA 1MG</t>
+  </si>
+  <si>
+    <t>LEVOMEPROMAZINA 4% GOTAS</t>
+  </si>
+  <si>
+    <t>LIDOCAINA 2% C/ VASO CONSTRITO</t>
+  </si>
+  <si>
+    <t>NITRATO DE CERIO +SULFADIAZINA</t>
+  </si>
+  <si>
+    <t>COLAGENASE+CLORAFENICOL POMADA 30g</t>
+  </si>
+  <si>
+    <t>RISPERIDONA</t>
+  </si>
+  <si>
+    <t>levomepromazina</t>
+  </si>
+  <si>
+    <t>LIDOCAÍNA</t>
+  </si>
+  <si>
+    <t>NITRATO DE CERIO;SULFADIAZINA</t>
+  </si>
+  <si>
+    <t>COLAGENASE</t>
+  </si>
+  <si>
+    <t>3mg</t>
+  </si>
+  <si>
+    <t>1mg</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>Concentração não encontrada</t>
+  </si>
+  <si>
+    <t>30g</t>
+  </si>
+  <si>
+    <t>Vitamedic</t>
+  </si>
+  <si>
+    <t>Sanofi</t>
+  </si>
+  <si>
+    <t>Cristália</t>
+  </si>
+  <si>
+    <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
+  </si>
+  <si>
+    <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
   </si>
 </sst>
 </file>
@@ -425,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,82 +498,122 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: CheckpointManager and add checkpointing to get_candidate_data
</commit_message>
<xml_diff>
--- a/relatorio_proc_dados.xlsx
+++ b/relatorio_proc_dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -40,73 +40,34 @@
     <t>PDF</t>
   </si>
   <si>
-    <t>RISPERIDONA 3MG</t>
-  </si>
-  <si>
-    <t>RISPERIDONA 1MG</t>
-  </si>
-  <si>
-    <t>LEVOMEPROMAZINA 4% GOTAS</t>
-  </si>
-  <si>
-    <t>LIDOCAINA 2% C/ VASO CONSTRITO</t>
-  </si>
-  <si>
-    <t>NITRATO DE CERIO +SULFADIAZINA</t>
-  </si>
-  <si>
-    <t>COLAGENASE+CLORAFENICOL POMADA 30g</t>
-  </si>
-  <si>
-    <t>RISPERIDONA</t>
-  </si>
-  <si>
-    <t>levomepromazina</t>
-  </si>
-  <si>
-    <t>LIDOCAÍNA</t>
-  </si>
-  <si>
-    <t>NITRATO DE CERIO;SULFADIAZINA</t>
-  </si>
-  <si>
-    <t>COLAGENASE</t>
-  </si>
-  <si>
-    <t>3mg</t>
-  </si>
-  <si>
-    <t>1mg</t>
-  </si>
-  <si>
-    <t>4%</t>
-  </si>
-  <si>
-    <t>2%</t>
-  </si>
-  <si>
-    <t>Concentração não encontrada</t>
-  </si>
-  <si>
-    <t>30g</t>
-  </si>
-  <si>
-    <t>Vitamedic</t>
-  </si>
-  <si>
-    <t>Sanofi</t>
-  </si>
-  <si>
-    <t>Cristália</t>
-  </si>
-  <si>
-    <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
-  </si>
-  <si>
-    <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
-  </si>
-  <si>
-    <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+  </si>
+  <si>
+    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
+  </si>
+  <si>
+    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
+  </si>
+  <si>
+    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+  </si>
+  <si>
+    <t>CLORETO DE SÓDIO;GLICOSE</t>
+  </si>
+  <si>
+    <t>1000ml</t>
+  </si>
+  <si>
+    <t>250ml</t>
+  </si>
+  <si>
+    <t>500ml</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
   </si>
 </sst>
 </file>
@@ -464,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,122 +459,82 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
         <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>